<commit_message>
generate excel file in resources
</commit_message>
<xml_diff>
--- a/src/main/resources/gasData.xlsx
+++ b/src/main/resources/gasData.xlsx
@@ -535,7 +535,7 @@
         <v>348.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -546,7 +546,7 @@
         <v>376.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5">
@@ -557,7 +557,7 @@
         <v>383.0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="6">
@@ -568,7 +568,7 @@
         <v>383.0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
@@ -579,7 +579,7 @@
         <v>396.0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
@@ -590,7 +590,7 @@
         <v>398.0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
@@ -601,7 +601,7 @@
         <v>408.0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -612,7 +612,7 @@
         <v>413.0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="11">
@@ -623,7 +623,7 @@
         <v>418.0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="12">
@@ -634,7 +634,7 @@
         <v>422.0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="13">
@@ -645,7 +645,7 @@
         <v>427.0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="14">
@@ -656,7 +656,7 @@
         <v>432.0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="15">
@@ -667,7 +667,7 @@
         <v>436.0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="16">
@@ -678,7 +678,7 @@
         <v>439.0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="17">
@@ -689,7 +689,7 @@
         <v>444.0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="18">
@@ -700,7 +700,7 @@
         <v>446.0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="19">
@@ -711,7 +711,7 @@
         <v>451.0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="20">
@@ -722,7 +722,7 @@
         <v>455.0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="21">
@@ -733,7 +733,7 @@
         <v>466.0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="22">
@@ -744,7 +744,7 @@
         <v>477.0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="23">
@@ -755,7 +755,7 @@
         <v>481.0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24">
@@ -766,7 +766,7 @@
         <v>485.0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="25">
@@ -777,7 +777,7 @@
         <v>495.0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="26">
@@ -788,7 +788,7 @@
         <v>498.0</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="27">
@@ -799,7 +799,7 @@
         <v>503.0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="28">
@@ -821,7 +821,7 @@
         <v>510.0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="30">
@@ -843,7 +843,7 @@
         <v>519.0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="32">
@@ -854,7 +854,7 @@
         <v>523.0</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="33">
@@ -865,7 +865,7 @@
         <v>527.0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="34">
@@ -876,7 +876,7 @@
         <v>532.0</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="35">
@@ -887,7 +887,7 @@
         <v>538.0</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="36">
@@ -898,7 +898,7 @@
         <v>542.0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="37">
@@ -909,7 +909,7 @@
         <v>545.0</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="38">
@@ -920,7 +920,7 @@
         <v>548.0</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="39">
@@ -931,7 +931,7 @@
         <v>555.0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="40">
@@ -942,7 +942,7 @@
         <v>559.0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="41">
@@ -953,7 +953,7 @@
         <v>565.0</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="42">
@@ -964,7 +964,7 @@
         <v>576.0</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="43">
@@ -975,7 +975,7 @@
         <v>581.0</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
@@ -986,7 +986,7 @@
         <v>585.0</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="45">
@@ -997,7 +997,7 @@
         <v>590.0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="46">
@@ -1008,7 +1008,7 @@
         <v>594.0</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="47">
@@ -1019,7 +1019,7 @@
         <v>601.0</v>
       </c>
       <c r="D47" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="48">
@@ -1030,7 +1030,7 @@
         <v>607.0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="49">
@@ -1041,7 +1041,7 @@
         <v>611.0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="50">
@@ -1052,7 +1052,7 @@
         <v>622.0</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="51">
@@ -1063,7 +1063,7 @@
         <v>626.0</v>
       </c>
       <c r="D51" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="52">
@@ -1074,7 +1074,7 @@
         <v>630.0</v>
       </c>
       <c r="D52" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="53">
@@ -1085,7 +1085,7 @@
         <v>644.0</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="54">
@@ -1096,7 +1096,7 @@
         <v>648.0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="55">
@@ -1107,7 +1107,7 @@
         <v>652.0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="56">
@@ -1118,7 +1118,7 @@
         <v>659.0</v>
       </c>
       <c r="D56" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="57">
@@ -1140,7 +1140,7 @@
         <v>667.0</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="59">
@@ -1151,7 +1151,7 @@
         <v>678.0</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="60">
@@ -1162,7 +1162,7 @@
         <v>678.0</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="61">
@@ -1173,7 +1173,7 @@
         <v>688.0</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="62">
@@ -1184,7 +1184,7 @@
         <v>695.0</v>
       </c>
       <c r="D62" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="63">
@@ -1195,7 +1195,7 @@
         <v>697.0</v>
       </c>
       <c r="D63" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="64">
@@ -1206,7 +1206,7 @@
         <v>701.0</v>
       </c>
       <c r="D64" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="65">
@@ -1217,7 +1217,7 @@
         <v>708.0</v>
       </c>
       <c r="D65" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="66">
@@ -1228,7 +1228,7 @@
         <v>711.0</v>
       </c>
       <c r="D66" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="67">
@@ -1239,7 +1239,7 @@
         <v>712.0</v>
       </c>
       <c r="D67" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="68">
@@ -1250,7 +1250,7 @@
         <v>715.0</v>
       </c>
       <c r="D68" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="69">
@@ -1261,7 +1261,7 @@
         <v>718.0</v>
       </c>
       <c r="D69" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="70">
@@ -1272,7 +1272,7 @@
         <v>728.0</v>
       </c>
       <c r="D70" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="71">
@@ -1283,7 +1283,7 @@
         <v>731.0</v>
       </c>
       <c r="D71" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="72">
@@ -1294,7 +1294,7 @@
         <v>734.0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="73">
@@ -1305,7 +1305,7 @@
         <v>739.0</v>
       </c>
       <c r="D73" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="74">
@@ -1316,7 +1316,7 @@
         <v>741.0</v>
       </c>
       <c r="D74" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="75">
@@ -1327,7 +1327,7 @@
         <v>745.0</v>
       </c>
       <c r="D75" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="76">
@@ -1338,7 +1338,7 @@
         <v>755.0</v>
       </c>
       <c r="D76" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="77">
@@ -1349,7 +1349,7 @@
         <v>758.0</v>
       </c>
       <c r="D77" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="78">
@@ -1360,7 +1360,7 @@
         <v>762.0</v>
       </c>
       <c r="D78" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="79">
@@ -1371,7 +1371,7 @@
         <v>766.0</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="80">
@@ -1382,7 +1382,7 @@
         <v>768.0</v>
       </c>
       <c r="D80" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="81">
@@ -1393,7 +1393,7 @@
         <v>771.0</v>
       </c>
       <c r="D81" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="82">
@@ -1404,7 +1404,7 @@
         <v>781.0</v>
       </c>
       <c r="D82" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="83">
@@ -1415,7 +1415,7 @@
         <v>785.0</v>
       </c>
       <c r="D83" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="84">
@@ -1426,7 +1426,7 @@
         <v>789.0</v>
       </c>
       <c r="D84" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="85">
@@ -1437,7 +1437,7 @@
         <v>791.0</v>
       </c>
       <c r="D85" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="86">
@@ -1448,7 +1448,7 @@
         <v>798.0</v>
       </c>
       <c r="D86" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="87">
@@ -1459,7 +1459,7 @@
         <v>799.0</v>
       </c>
       <c r="D87" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="88">
@@ -1470,7 +1470,7 @@
         <v>802.0</v>
       </c>
       <c r="D88" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="89">
@@ -1481,7 +1481,7 @@
         <v>807.0</v>
       </c>
       <c r="D89" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="90">
@@ -1492,7 +1492,7 @@
         <v>809.0</v>
       </c>
       <c r="D90" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="91">
@@ -1503,7 +1503,7 @@
         <v>811.0</v>
       </c>
       <c r="D91" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="92">
@@ -1525,7 +1525,7 @@
         <v>813.0</v>
       </c>
       <c r="D93" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="94">
@@ -1536,7 +1536,7 @@
         <v>813.0</v>
       </c>
       <c r="D94" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="95">
@@ -1547,7 +1547,7 @@
         <v>814.0</v>
       </c>
       <c r="D95" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="96">
@@ -1558,7 +1558,7 @@
         <v>816.0</v>
       </c>
       <c r="D96" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="97">
@@ -1569,7 +1569,7 @@
         <v>817.0</v>
       </c>
       <c r="D97" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="98">
@@ -1580,7 +1580,7 @@
         <v>820.0</v>
       </c>
       <c r="D98" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="99">
@@ -1591,7 +1591,7 @@
         <v>820.0</v>
       </c>
       <c r="D99" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="100">
@@ -1602,7 +1602,7 @@
         <v>822.0</v>
       </c>
       <c r="D100" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="101">
@@ -1613,7 +1613,7 @@
         <v>827.0</v>
       </c>
       <c r="D101" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="102">
@@ -1624,7 +1624,7 @@
         <v>830.0</v>
       </c>
       <c r="D102" t="n">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="103">
@@ -1635,7 +1635,7 @@
         <v>844.0</v>
       </c>
       <c r="D103" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="104">
@@ -1646,7 +1646,7 @@
         <v>847.0</v>
       </c>
       <c r="D104" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="105">
@@ -1657,7 +1657,7 @@
         <v>849.0</v>
       </c>
       <c r="D105" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="106">
@@ -1668,7 +1668,7 @@
         <v>850.0</v>
       </c>
       <c r="D106" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="107">
@@ -1679,7 +1679,7 @@
         <v>851.0</v>
       </c>
       <c r="D107" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="108">
@@ -1690,7 +1690,7 @@
         <v>854.0</v>
       </c>
       <c r="D108" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="109">
@@ -1701,7 +1701,7 @@
         <v>855.0</v>
       </c>
       <c r="D109" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="110">
@@ -1712,7 +1712,7 @@
         <v>858.0</v>
       </c>
       <c r="D110" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="111">
@@ -1723,7 +1723,7 @@
         <v>866.0</v>
       </c>
       <c r="D111" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="112">
@@ -1734,7 +1734,7 @@
         <v>872.0</v>
       </c>
       <c r="D112" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="113">
@@ -1745,7 +1745,7 @@
         <v>874.0</v>
       </c>
       <c r="D113" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="114">
@@ -1756,7 +1756,7 @@
         <v>884.0</v>
       </c>
       <c r="D114" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="115">
@@ -1767,7 +1767,7 @@
         <v>897.0</v>
       </c>
       <c r="D115" t="n">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="116">
@@ -1778,7 +1778,7 @@
         <v>922.0</v>
       </c>
       <c r="D116" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="117">
@@ -1789,7 +1789,7 @@
         <v>942.0</v>
       </c>
       <c r="D117" t="n">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="118">
@@ -1800,7 +1800,7 @@
         <v>950.0</v>
       </c>
       <c r="D118" t="n">
-        <v>0.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="119">
@@ -1811,7 +1811,7 @@
         <v>962.0</v>
       </c>
       <c r="D119" t="n">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="120">
@@ -1822,7 +1822,7 @@
         <v>970.0</v>
       </c>
       <c r="D120" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="121">
@@ -1833,7 +1833,7 @@
         <v>970.0</v>
       </c>
       <c r="D121" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="122">
@@ -1844,7 +1844,7 @@
         <v>1062.0</v>
       </c>
       <c r="D122" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="123">
@@ -1855,7 +1855,7 @@
         <v>1089.0</v>
       </c>
       <c r="D123" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="124">
@@ -1866,7 +1866,7 @@
         <v>1102.0</v>
       </c>
       <c r="D124" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="125">
@@ -1877,7 +1877,7 @@
         <v>1109.0</v>
       </c>
       <c r="D125" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="126">
@@ -1888,7 +1888,7 @@
         <v>1158.0</v>
       </c>
       <c r="D126" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="127">
@@ -1899,7 +1899,7 @@
         <v>1185.0</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="128">
@@ -1910,7 +1910,7 @@
         <v>1190.0</v>
       </c>
       <c r="D128" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="129">
@@ -1921,7 +1921,7 @@
         <v>1231.0</v>
       </c>
       <c r="D129" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="130">
@@ -1932,7 +1932,7 @@
         <v>1263.0</v>
       </c>
       <c r="D130" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="131">
@@ -1943,7 +1943,7 @@
         <v>1294.0</v>
       </c>
       <c r="D131" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="132">
@@ -1954,7 +1954,7 @@
         <v>1347.0</v>
       </c>
       <c r="D132" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="133">
@@ -1965,7 +1965,7 @@
         <v>1390.0</v>
       </c>
       <c r="D133" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="134">
@@ -1976,7 +1976,7 @@
         <v>1422.0</v>
       </c>
       <c r="D134" t="n">
-        <v>0.0</v>
+        <v>-4.0</v>
       </c>
     </row>
     <row r="135">
@@ -1987,7 +1987,7 @@
         <v>1470.0</v>
       </c>
       <c r="D135" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="136">
@@ -1998,7 +1998,7 @@
         <v>1513.0</v>
       </c>
       <c r="D136" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="137">
@@ -2009,7 +2009,7 @@
         <v>1556.0</v>
       </c>
       <c r="D137" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="138">
@@ -2020,7 +2020,7 @@
         <v>1680.0</v>
       </c>
       <c r="D138" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="139">
@@ -2031,7 +2031,7 @@
         <v>1706.0</v>
       </c>
       <c r="D139" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="140">
@@ -2042,7 +2042,7 @@
         <v>1744.0</v>
       </c>
       <c r="D140" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="141">
@@ -2053,7 +2053,7 @@
         <v>1768.0</v>
       </c>
       <c r="D141" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="142">
@@ -2064,7 +2064,7 @@
         <v>1798.0</v>
       </c>
       <c r="D142" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="143">
@@ -2075,7 +2075,7 @@
         <v>1846.0</v>
       </c>
       <c r="D143" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="144">
@@ -2086,7 +2086,7 @@
         <v>1872.0</v>
       </c>
       <c r="D144" t="n">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="145">
@@ -2097,7 +2097,7 @@
         <v>1937.0</v>
       </c>
       <c r="D145" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="146">
@@ -2108,7 +2108,7 @@
         <v>1978.0</v>
       </c>
       <c r="D146" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="147">
@@ -2119,7 +2119,7 @@
         <v>2032.0</v>
       </c>
       <c r="D147" t="n">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="148">
@@ -2130,7 +2130,7 @@
         <v>2040.0</v>
       </c>
       <c r="D148" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="149" ht="35.0" customHeight="true">
@@ -2178,7 +2178,7 @@
         <v>348.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -2189,7 +2189,7 @@
         <v>376.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5">
@@ -2200,7 +2200,7 @@
         <v>383.0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="6">
@@ -2211,7 +2211,7 @@
         <v>383.0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
@@ -2222,7 +2222,7 @@
         <v>396.0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
@@ -2233,7 +2233,7 @@
         <v>398.0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
@@ -2244,7 +2244,7 @@
         <v>408.0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -2255,7 +2255,7 @@
         <v>413.0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="11">
@@ -2266,7 +2266,7 @@
         <v>418.0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="12">
@@ -2277,7 +2277,7 @@
         <v>422.0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="13">
@@ -2288,7 +2288,7 @@
         <v>427.0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="14">
@@ -2299,7 +2299,7 @@
         <v>432.0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="15">
@@ -2310,7 +2310,7 @@
         <v>436.0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="16">
@@ -2321,7 +2321,7 @@
         <v>439.0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="17">
@@ -2332,7 +2332,7 @@
         <v>444.0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="18">
@@ -2343,7 +2343,7 @@
         <v>446.0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="19">
@@ -2354,7 +2354,7 @@
         <v>451.0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="20">
@@ -2365,7 +2365,7 @@
         <v>455.0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="21">
@@ -2376,7 +2376,7 @@
         <v>466.0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="22">
@@ -2387,7 +2387,7 @@
         <v>477.0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="23">
@@ -2398,7 +2398,7 @@
         <v>481.0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24">
@@ -2409,7 +2409,7 @@
         <v>485.0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="25" ht="35.0" customHeight="true">
@@ -2457,7 +2457,7 @@
         <v>1390.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="4">
@@ -2468,7 +2468,7 @@
         <v>1422.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>-4.0</v>
       </c>
     </row>
     <row r="5">
@@ -2479,7 +2479,7 @@
         <v>1470.0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="6">
@@ -2490,7 +2490,7 @@
         <v>1513.0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="7">
@@ -2501,7 +2501,7 @@
         <v>1556.0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="8">
@@ -2512,7 +2512,7 @@
         <v>1680.0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="9">
@@ -2523,7 +2523,7 @@
         <v>1706.0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -2534,7 +2534,7 @@
         <v>1744.0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="11">
@@ -2545,7 +2545,7 @@
         <v>1768.0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="12">
@@ -2556,7 +2556,7 @@
         <v>1798.0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="13">
@@ -2567,7 +2567,7 @@
         <v>1846.0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="14">
@@ -2578,7 +2578,7 @@
         <v>1872.0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="15">
@@ -2589,7 +2589,7 @@
         <v>1937.0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -2600,7 +2600,7 @@
         <v>1978.0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="17">
@@ -2611,7 +2611,7 @@
         <v>2032.0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="18">
@@ -2622,7 +2622,7 @@
         <v>2040.0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="19" ht="35.0" customHeight="true">
@@ -2670,7 +2670,7 @@
         <v>495.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
@@ -2681,7 +2681,7 @@
         <v>498.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="5">
@@ -2692,7 +2692,7 @@
         <v>503.0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
@@ -2714,7 +2714,7 @@
         <v>510.0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="8">
@@ -2736,7 +2736,7 @@
         <v>519.0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -2747,7 +2747,7 @@
         <v>523.0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">
@@ -2758,7 +2758,7 @@
         <v>527.0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="12">
@@ -2769,7 +2769,7 @@
         <v>532.0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="13">
@@ -2780,7 +2780,7 @@
         <v>538.0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="14">
@@ -2791,7 +2791,7 @@
         <v>542.0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="15">
@@ -2802,7 +2802,7 @@
         <v>545.0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="16">
@@ -2813,7 +2813,7 @@
         <v>548.0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="17">
@@ -2824,7 +2824,7 @@
         <v>555.0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="18">
@@ -2835,7 +2835,7 @@
         <v>559.0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="19">
@@ -2846,7 +2846,7 @@
         <v>565.0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
@@ -2857,7 +2857,7 @@
         <v>576.0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="21">
@@ -2868,7 +2868,7 @@
         <v>581.0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="22">
@@ -2879,7 +2879,7 @@
         <v>585.0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="23">
@@ -2890,7 +2890,7 @@
         <v>590.0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24">
@@ -2901,7 +2901,7 @@
         <v>594.0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="25">
@@ -2912,7 +2912,7 @@
         <v>601.0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="26">
@@ -2923,7 +2923,7 @@
         <v>607.0</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="27">
@@ -2934,7 +2934,7 @@
         <v>611.0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28">
@@ -2945,7 +2945,7 @@
         <v>622.0</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="29">
@@ -2956,7 +2956,7 @@
         <v>626.0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="30">
@@ -2967,7 +2967,7 @@
         <v>630.0</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="31">
@@ -2978,7 +2978,7 @@
         <v>644.0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="32">
@@ -2989,7 +2989,7 @@
         <v>648.0</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="33">
@@ -3000,7 +3000,7 @@
         <v>652.0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="34">
@@ -3011,7 +3011,7 @@
         <v>659.0</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="35">
@@ -3033,7 +3033,7 @@
         <v>667.0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="37">
@@ -3044,7 +3044,7 @@
         <v>678.0</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="38">
@@ -3055,7 +3055,7 @@
         <v>678.0</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="39">
@@ -3066,7 +3066,7 @@
         <v>688.0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="40">
@@ -3077,7 +3077,7 @@
         <v>695.0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="41">
@@ -3088,7 +3088,7 @@
         <v>697.0</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="42">
@@ -3099,7 +3099,7 @@
         <v>701.0</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="43">
@@ -3110,7 +3110,7 @@
         <v>708.0</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="44">
@@ -3121,7 +3121,7 @@
         <v>711.0</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="45">
@@ -3132,7 +3132,7 @@
         <v>712.0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="46">
@@ -3143,7 +3143,7 @@
         <v>715.0</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="47">
@@ -3154,7 +3154,7 @@
         <v>718.0</v>
       </c>
       <c r="D47" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="48">
@@ -3165,7 +3165,7 @@
         <v>728.0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="49">
@@ -3176,7 +3176,7 @@
         <v>731.0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="50">
@@ -3187,7 +3187,7 @@
         <v>734.0</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="51">
@@ -3198,7 +3198,7 @@
         <v>739.0</v>
       </c>
       <c r="D51" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="52">
@@ -3209,7 +3209,7 @@
         <v>741.0</v>
       </c>
       <c r="D52" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="53">
@@ -3220,7 +3220,7 @@
         <v>745.0</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="54">
@@ -3231,7 +3231,7 @@
         <v>755.0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="55">
@@ -3242,7 +3242,7 @@
         <v>758.0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="56">
@@ -3253,7 +3253,7 @@
         <v>762.0</v>
       </c>
       <c r="D56" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="57">
@@ -3264,7 +3264,7 @@
         <v>766.0</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="58">
@@ -3275,7 +3275,7 @@
         <v>768.0</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="59">
@@ -3286,7 +3286,7 @@
         <v>771.0</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="60">
@@ -3297,7 +3297,7 @@
         <v>781.0</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="61">
@@ -3308,7 +3308,7 @@
         <v>785.0</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="62">
@@ -3319,7 +3319,7 @@
         <v>789.0</v>
       </c>
       <c r="D62" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="63">
@@ -3330,7 +3330,7 @@
         <v>791.0</v>
       </c>
       <c r="D63" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="64">
@@ -3341,7 +3341,7 @@
         <v>798.0</v>
       </c>
       <c r="D64" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="65">
@@ -3352,7 +3352,7 @@
         <v>799.0</v>
       </c>
       <c r="D65" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="66">
@@ -3363,7 +3363,7 @@
         <v>802.0</v>
       </c>
       <c r="D66" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="67">
@@ -3374,7 +3374,7 @@
         <v>807.0</v>
       </c>
       <c r="D67" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="68">
@@ -3385,7 +3385,7 @@
         <v>809.0</v>
       </c>
       <c r="D68" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="69">
@@ -3396,7 +3396,7 @@
         <v>811.0</v>
       </c>
       <c r="D69" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="70">
@@ -3418,7 +3418,7 @@
         <v>813.0</v>
       </c>
       <c r="D71" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="72">
@@ -3429,7 +3429,7 @@
         <v>813.0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="73">
@@ -3440,7 +3440,7 @@
         <v>814.0</v>
       </c>
       <c r="D73" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="74">
@@ -3451,7 +3451,7 @@
         <v>816.0</v>
       </c>
       <c r="D74" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="75">
@@ -3462,7 +3462,7 @@
         <v>817.0</v>
       </c>
       <c r="D75" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="76">
@@ -3473,7 +3473,7 @@
         <v>820.0</v>
       </c>
       <c r="D76" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="77">
@@ -3484,7 +3484,7 @@
         <v>820.0</v>
       </c>
       <c r="D77" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="78">
@@ -3495,7 +3495,7 @@
         <v>822.0</v>
       </c>
       <c r="D78" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="79">
@@ -3506,7 +3506,7 @@
         <v>827.0</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="80">
@@ -3517,7 +3517,7 @@
         <v>830.0</v>
       </c>
       <c r="D80" t="n">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="81">
@@ -3528,7 +3528,7 @@
         <v>844.0</v>
       </c>
       <c r="D81" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="82">
@@ -3539,7 +3539,7 @@
         <v>847.0</v>
       </c>
       <c r="D82" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="83">
@@ -3550,7 +3550,7 @@
         <v>849.0</v>
       </c>
       <c r="D83" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="84">
@@ -3561,7 +3561,7 @@
         <v>850.0</v>
       </c>
       <c r="D84" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="85">
@@ -3572,7 +3572,7 @@
         <v>851.0</v>
       </c>
       <c r="D85" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="86">
@@ -3583,7 +3583,7 @@
         <v>854.0</v>
       </c>
       <c r="D86" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="87">
@@ -3594,7 +3594,7 @@
         <v>855.0</v>
       </c>
       <c r="D87" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="88">
@@ -3605,7 +3605,7 @@
         <v>858.0</v>
       </c>
       <c r="D88" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="89">
@@ -3616,7 +3616,7 @@
         <v>866.0</v>
       </c>
       <c r="D89" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="90">
@@ -3627,7 +3627,7 @@
         <v>872.0</v>
       </c>
       <c r="D90" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="91">
@@ -3638,7 +3638,7 @@
         <v>874.0</v>
       </c>
       <c r="D91" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="92">
@@ -3649,7 +3649,7 @@
         <v>884.0</v>
       </c>
       <c r="D92" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="93">
@@ -3660,7 +3660,7 @@
         <v>897.0</v>
       </c>
       <c r="D93" t="n">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="94">
@@ -3671,7 +3671,7 @@
         <v>922.0</v>
       </c>
       <c r="D94" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="95">
@@ -3682,7 +3682,7 @@
         <v>942.0</v>
       </c>
       <c r="D95" t="n">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="96">
@@ -3693,7 +3693,7 @@
         <v>950.0</v>
       </c>
       <c r="D96" t="n">
-        <v>0.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="97">
@@ -3704,7 +3704,7 @@
         <v>962.0</v>
       </c>
       <c r="D97" t="n">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="98">
@@ -3715,7 +3715,7 @@
         <v>970.0</v>
       </c>
       <c r="D98" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="99">
@@ -3726,7 +3726,7 @@
         <v>970.0</v>
       </c>
       <c r="D99" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="100">
@@ -3737,7 +3737,7 @@
         <v>1062.0</v>
       </c>
       <c r="D100" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="101">
@@ -3748,7 +3748,7 @@
         <v>1089.0</v>
       </c>
       <c r="D101" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="102">
@@ -3759,7 +3759,7 @@
         <v>1102.0</v>
       </c>
       <c r="D102" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="103">
@@ -3770,7 +3770,7 @@
         <v>1109.0</v>
       </c>
       <c r="D103" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="104">
@@ -3781,7 +3781,7 @@
         <v>1158.0</v>
       </c>
       <c r="D104" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="105">
@@ -3792,7 +3792,7 @@
         <v>1185.0</v>
       </c>
       <c r="D105" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="106">
@@ -3803,7 +3803,7 @@
         <v>1190.0</v>
       </c>
       <c r="D106" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="107">
@@ -3814,7 +3814,7 @@
         <v>1231.0</v>
       </c>
       <c r="D107" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="108">
@@ -3825,7 +3825,7 @@
         <v>1263.0</v>
       </c>
       <c r="D108" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="109">
@@ -3836,7 +3836,7 @@
         <v>1294.0</v>
       </c>
       <c r="D109" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="110">
@@ -3847,7 +3847,7 @@
         <v>1347.0</v>
       </c>
       <c r="D110" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="111" ht="35.0" customHeight="true">

</xml_diff>